<commit_message>
scripts NZO and C57 and echoMRI
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz03072025.xlsx
+++ b/data/echoMRI/Kotz03072025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBAA221-3CB8-E342-BA52-C183D434807F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDDB53F-AC9D-0143-B521-4A350B7C2C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="22780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedScans" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>RecNumber</t>
   </si>
@@ -553,7 +553,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -1264,8 +1264,8 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>17</v>
+      <c r="B25">
+        <v>7873</v>
       </c>
       <c r="C25">
         <v>1.36</v>

</xml_diff>

<commit_message>
NZO and C57 TEE
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz03072025.xlsx
+++ b/data/echoMRI/Kotz03072025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDDB53F-AC9D-0143-B521-4A350B7C2C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2553A2FE-D4E9-6341-BB70-14DFA76A4B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="22780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -1265,7 +1265,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>7873</v>
+        <v>7883</v>
       </c>
       <c r="C25">
         <v>1.36</v>

</xml_diff>